<commit_message>
edits to synchronize search requests
</commit_message>
<xml_diff>
--- a/GoogleSearchResults.xlsx
+++ b/GoogleSearchResults.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="312">
   <si>
     <t>Google search results for: Mobile ad firm</t>
   </si>
@@ -44,30 +44,30 @@
     <t>https://blog.hubspot.com/agency/mobile-advertising-companies</t>
   </si>
   <si>
+    <t>The top 10 mobile advertising companies | VentureBeat | Mobile | by ...</t>
+  </si>
+  <si>
+    <t>https://venturebeat.com/2013/06/12/the-top-10-mobile-advertising-companies/</t>
+  </si>
+  <si>
+    <t>Mobile Advertising for Brands, Agencies and Performance Marketers</t>
+  </si>
+  <si>
+    <t>http://www.millennialmedia.com/solutions/advertiser</t>
+  </si>
+  <si>
+    <t>Mobile Advertising and App Monetization Platform</t>
+  </si>
+  <si>
+    <t>http://www.millennialmedia.com/</t>
+  </si>
+  <si>
     <t>mobile advertising | TechCrunch</t>
   </si>
   <si>
     <t>https://techcrunch.com/tag/mobile-advertising/</t>
   </si>
   <si>
-    <t>The top 10 mobile advertising companies | VentureBeat | Mobile | by ...</t>
-  </si>
-  <si>
-    <t>https://venturebeat.com/2013/06/12/the-top-10-mobile-advertising-companies/</t>
-  </si>
-  <si>
-    <t>Mobile Advertising for Brands, Agencies and Performance Marketers</t>
-  </si>
-  <si>
-    <t>http://www.millennialmedia.com/solutions/advertiser</t>
-  </si>
-  <si>
-    <t>Mobile Advertising and App Monetization Platform</t>
-  </si>
-  <si>
-    <t>http://www.millennialmedia.com/</t>
-  </si>
-  <si>
     <t>Mobile Ad Firm Verve Acquires Beacon Company Roximity - WSJ</t>
   </si>
   <si>
@@ -98,30 +98,30 @@
     <t>https://qz.com/714905/the-us-has-fined-mobile-ads-firm-inmobi-for-tracking-the-location-of-hundreds-of-millions-of-people/</t>
   </si>
   <si>
+    <t>Mobile Advertising | User Acquisition | Game Marketing | App Installs</t>
+  </si>
+  <si>
+    <t>http://motiveinteractive.com/</t>
+  </si>
+  <si>
     <t>Airpush: Mobile Ad Network | Android App Monetization</t>
   </si>
   <si>
     <t>http://www.airpush.com/</t>
   </si>
   <si>
+    <t>AdColony - Elevating mobile advertising across today's hottest apps</t>
+  </si>
+  <si>
+    <t>https://www.adcolony.com/</t>
+  </si>
+  <si>
     <t>xAd - Location-Based Marketing, Without The Guesswork</t>
   </si>
   <si>
     <t>http://www.xad.com/</t>
   </si>
   <si>
-    <t>AdColony - Elevating mobile advertising across today's hottest apps</t>
-  </si>
-  <si>
-    <t>https://www.adcolony.com/</t>
-  </si>
-  <si>
-    <t>Mobile Advertising | User Acquisition | Game Marketing | App Installs</t>
-  </si>
-  <si>
-    <t>http://motiveinteractive.com/</t>
-  </si>
-  <si>
     <t>Mobile advertising - Wikipedia</t>
   </si>
   <si>
@@ -140,6 +140,12 @@
     <t>https://pingmobile.com/</t>
   </si>
   <si>
+    <t>Red Square Agency</t>
+  </si>
+  <si>
+    <t>http://www.redsquareagency.com/</t>
+  </si>
+  <si>
     <t>Qualcomm spin-off Gimbal acquired by LA mobile ad firm - The San ...</t>
   </si>
   <si>
@@ -158,24 +164,30 @@
     <t>https://www.crunchbase.com/organization/kargo</t>
   </si>
   <si>
+    <t>Singapore mobile ad firm fined $950 K for 'deceptively' tracking - ZDNet</t>
+  </si>
+  <si>
+    <t>http://www.zdnet.com/article/singapore-mobile-ad-firm-fined-950k-for-deceptively-tracking-consumer-location/</t>
+  </si>
+  <si>
     <t>Mobile Advertising Agency | Bamboo - Direct Response Ad Agency in ...</t>
   </si>
   <si>
     <t>http://www.growwithbamboo.com/</t>
   </si>
   <si>
-    <t>Singapore mobile ad firm fined $950 K for 'deceptively' tracking - ZDNet</t>
-  </si>
-  <si>
-    <t>http://www.zdnet.com/article/singapore-mobile-ad-firm-fined-950k-for-deceptively-tracking-consumer-location/</t>
-  </si>
-  <si>
     <t>Widespace | Technology to build brands in a mobile world</t>
   </si>
   <si>
     <t>https://www.widespace.com/</t>
   </si>
   <si>
+    <t>Top 9 Best-Paying Mobile Ad Networks You Should Try - AdPushup</t>
+  </si>
+  <si>
+    <t>https://www.adpushup.com/blog/top-8-best-paying-mobile-ad-networks-you-should-try/</t>
+  </si>
+  <si>
     <t>Beacon Maker Gimbal Acquired By Mobile Advertising Firm 12/05/2016</t>
   </si>
   <si>
@@ -254,6 +266,66 @@
     <t>http://fortune.com/2016/06/22/ad-tracking-fine/</t>
   </si>
   <si>
+    <t>Optimization Issues in Web and Mobile Advertising: Past and Future ...</t>
+  </si>
+  <si>
+    <t>https://books.google.com/books?id=u_LuCgAAQBAJ&amp;pg=PA41&amp;lpg=PA41&amp;dq=Mobile+ad+firm&amp;source=bl&amp;ots=SNDZ72jn95&amp;sig=EnFW3mrYjSE1He2-F4qISQoKnkQ&amp;hl=en&amp;sa=X&amp;ved=0ahUKEwiB5Ybto7zTAhXHWSYKHShfBWA4KBDoAQgjMAA</t>
+  </si>
+  <si>
+    <t>Chinese Investors Inject $100M In Mobile Advertising Firm Yeahmobi ...</t>
+  </si>
+  <si>
+    <t>https://www.chinamoneynetwork.com/2016/12/21/chinese-investors-inject-100m-in-mobile-advertising-firm-yeahmobi</t>
+  </si>
+  <si>
+    <t>Singapore-based mobile ad firm BuzzCity acquired by Mobads ...</t>
+  </si>
+  <si>
+    <t>http://lovelymobile.news/singapore-based-mobile-ad-firm-buzzcity-acquired-by-mobads/</t>
+  </si>
+  <si>
+    <t>Amobee: Home</t>
+  </si>
+  <si>
+    <t>http://www.amobee.com/</t>
+  </si>
+  <si>
+    <t>Mobile ad firm moving at rapid rate « Zapis Capital Portfolio</t>
+  </si>
+  <si>
+    <t>http://zapiscapital.com/news/mobile-ad-firm-moving-at-rapid-rate/</t>
+  </si>
+  <si>
+    <t>Medialets</t>
+  </si>
+  <si>
+    <t>https://www.medialets.com/</t>
+  </si>
+  <si>
+    <t>Marchex: Transform Mobile Advertising Performance</t>
+  </si>
+  <si>
+    <t>http://www.marchex.com/</t>
+  </si>
+  <si>
+    <t>Hipcricket®</t>
+  </si>
+  <si>
+    <t>https://www.hipcricket.com/</t>
+  </si>
+  <si>
+    <t>Chinese mobile ad firm accused of distributing Android malware ...</t>
+  </si>
+  <si>
+    <t>http://www.marketing-interactive.com/chinese-mobile-ad-firm-accused-of-distributing-android-malware/</t>
+  </si>
+  <si>
+    <t>Pinterest confirms 'acqhire' of mobile advertising startup URX - Recode</t>
+  </si>
+  <si>
+    <t>https://www.recode.net/2016/5/3/11634202/pinterest-acqhire-advertising-urx</t>
+  </si>
+  <si>
     <t>Google search results for: Mobile advertising</t>
   </si>
   <si>
@@ -275,36 +347,36 @@
     <t>http://www.adweek.com/tag/mobile-advertising/</t>
   </si>
   <si>
+    <t>A blow for mobile advertising: The next version of Safari will let users ...</t>
+  </si>
+  <si>
+    <t>http://www.niemanlab.org/2015/06/a-blow-for-mobile-advertising-the-next-version-of-safari-will-let-users-block-ads-on-iphones-and-ipads/</t>
+  </si>
+  <si>
+    <t>For Mobile Devices, Think Apps, Not Ads - Harvard Business Review</t>
+  </si>
+  <si>
+    <t>https://hbr.org/2013/03/for-mobile-devices-think-apps-not-ads</t>
+  </si>
+  <si>
+    <t>Why Mobile Will Dominate the Future of Media and Advertising - The ...</t>
+  </si>
+  <si>
+    <t>https://www.theatlantic.com/business/archive/2012/06/why-mobile-will-dominate-the-future-of-media-and-advertising/258069/</t>
+  </si>
+  <si>
+    <t>What you need to know about the state of mobile advertising</t>
+  </si>
+  <si>
+    <t>http://marketingland.com/state-mobile-advertising-192061</t>
+  </si>
+  <si>
     <t>Demystifying the booming mobile advertising market | TechCrunch</t>
   </si>
   <si>
     <t>https://techcrunch.com/2016/08/06/demystifying-the-booming-mobile-advertising-market/</t>
   </si>
   <si>
-    <t>A blow for mobile advertising: The next version of Safari will let users ...</t>
-  </si>
-  <si>
-    <t>http://www.niemanlab.org/2015/06/a-blow-for-mobile-advertising-the-next-version-of-safari-will-let-users-block-ads-on-iphones-and-ipads/</t>
-  </si>
-  <si>
-    <t>For Mobile Devices, Think Apps, Not Ads - Harvard Business Review</t>
-  </si>
-  <si>
-    <t>https://hbr.org/2013/03/for-mobile-devices-think-apps-not-ads</t>
-  </si>
-  <si>
-    <t>Why Mobile Will Dominate the Future of Media and Advertising - The ...</t>
-  </si>
-  <si>
-    <t>https://www.theatlantic.com/business/archive/2012/06/why-mobile-will-dominate-the-future-of-media-and-advertising/258069/</t>
-  </si>
-  <si>
-    <t>What you need to know about the state of mobile advertising</t>
-  </si>
-  <si>
-    <t>http://marketingland.com/state-mobile-advertising-192061</t>
-  </si>
-  <si>
     <t>Mobile Advertising - Mashable</t>
   </si>
   <si>
@@ -347,12 +419,24 @@
     <t>https://gimbal.com/mobile-ad-types/</t>
   </si>
   <si>
+    <t>Supersonic: Mobile Advertising | App Monetization</t>
+  </si>
+  <si>
+    <t>https://www.supersonic.com/</t>
+  </si>
+  <si>
     <t>Mobile Advertising &amp; Freelance App Marketing Services | Fiverr</t>
   </si>
   <si>
     <t>https://www.fiverr.com/categories/online-marketing/mobile-advertising</t>
   </si>
   <si>
+    <t>Advertising Product Suite | Phunware Mobile Advertising</t>
+  </si>
+  <si>
+    <t>http://www.phunware.com/advertising/</t>
+  </si>
+  <si>
     <t>Mobile Advertising - ExactDrive</t>
   </si>
   <si>
@@ -365,10 +449,10 @@
     <t>https://www.doubleclickbygoogle.com/solutions/mobile/</t>
   </si>
   <si>
-    <t>Advertising Product Suite | Phunware Mobile Advertising</t>
-  </si>
-  <si>
-    <t>http://www.phunware.com/advertising/</t>
+    <t>What is Mobile Advertising - Know Online Advertising</t>
+  </si>
+  <si>
+    <t>http://www.knowonlineadvertising.com/online-mobile-advertising/</t>
   </si>
   <si>
     <t>Mobile Advertising Guidelines - Mobile Marketing Association</t>
@@ -377,66 +461,6 @@
     <t>http://www.mmaglobal.com/files/mobileadvertising.pdf</t>
   </si>
   <si>
-    <t>Best Mobile Advertising Software in 2017 | G2 Crowd</t>
-  </si>
-  <si>
-    <t>https://www.g2crowd.com/categories/mobile-advertising</t>
-  </si>
-  <si>
-    <t>Amazon Mobile Ad Network | Amazon Developer Portal</t>
-  </si>
-  <si>
-    <t>https://developer.amazon.com/mobile-ads</t>
-  </si>
-  <si>
-    <t>Mobile Advertising Startups - AngelList</t>
-  </si>
-  <si>
-    <t>https://angel.co/mobile-advertising</t>
-  </si>
-  <si>
-    <t>Mobile Advertising News &amp; Information | MobileAdvertisingWatch.com</t>
-  </si>
-  <si>
-    <t>http://mobileadvertisingwatch.com/</t>
-  </si>
-  <si>
-    <t>Sled Mobile: High-impact mobile advertising</t>
-  </si>
-  <si>
-    <t>http://www.sledmobile.com/</t>
-  </si>
-  <si>
-    <t>Mobile Advertising Solutions - Bing Ads</t>
-  </si>
-  <si>
-    <t>https://advertise.bingads.microsoft.com/en-us/solutions/mobile-advertising</t>
-  </si>
-  <si>
-    <t>Mobile Advertising &amp; Trends – Think with Google</t>
-  </si>
-  <si>
-    <t>https://www.thinkwithgoogle.com/topics/mobile-advertising-trends.html</t>
-  </si>
-  <si>
-    <t>Mobile Phone Creative Guidelines - IAB</t>
-  </si>
-  <si>
-    <t>https://www.iab.com/guidelines/mobile-phone-creative-guidelines/</t>
-  </si>
-  <si>
-    <t>Mobile Advertising - Immersion Corporation</t>
-  </si>
-  <si>
-    <t>https://www.immersion.com/mobile-advertising/</t>
-  </si>
-  <si>
-    <t>Matomy Media Group | Mobile Advertisers</t>
-  </si>
-  <si>
-    <t>http://www.matomy.com/mobile-advertisers/</t>
-  </si>
-  <si>
     <t>Google search results for: Mobile marketing</t>
   </si>
   <si>
@@ -476,48 +500,60 @@
     <t>http://mobilemarketingmagazine.com/</t>
   </si>
   <si>
+    <t>Mobile Marketing Definition | Investopedia</t>
+  </si>
+  <si>
+    <t>http://www.investopedia.com/terms/m/mobile-marketing.asp</t>
+  </si>
+  <si>
+    <t>What is mobile marketing? - Definition from WhatIs.com</t>
+  </si>
+  <si>
+    <t>http://searchmobilecomputing.techtarget.com/definition/mobile-marketing</t>
+  </si>
+  <si>
     <t>Mobile Marketing Watch: Home</t>
   </si>
   <si>
     <t>https://mobilemarketingwatch.com/</t>
   </si>
   <si>
-    <t>Mobile Marketing Definition | Investopedia</t>
-  </si>
-  <si>
-    <t>http://www.investopedia.com/terms/m/mobile-marketing.asp</t>
-  </si>
-  <si>
-    <t>What is mobile marketing? - Definition from WhatIs.com</t>
-  </si>
-  <si>
-    <t>http://searchmobilecomputing.techtarget.com/definition/mobile-marketing</t>
-  </si>
-  <si>
     <t>Mobile Marketing News &amp; Topics - Entrepreneur</t>
   </si>
   <si>
     <t>https://www.entrepreneur.com/topic/mobile-marketing</t>
   </si>
   <si>
+    <t>10 mobile marketing trends to watch in 2017 | CIO</t>
+  </si>
+  <si>
+    <t>http://www.cio.com/article/3174133/mobile/10-mobile-marketing-trends-to-watch-in-2017.html</t>
+  </si>
+  <si>
     <t>What is Mobile Marketing? - Business News Daily</t>
   </si>
   <si>
     <t>http://www.businessnewsdaily.com/4962-what-is-mobile-marketing.html</t>
   </si>
   <si>
-    <t>10 mobile marketing trends to watch in 2017 | CIO</t>
-  </si>
-  <si>
-    <t>http://www.cio.com/article/3174133/mobile/10-mobile-marketing-trends-to-watch-in-2017.html</t>
-  </si>
-  <si>
     <t>Mobile Marketer: News about marketing, apps, mobile video, mobile ...</t>
   </si>
   <si>
     <t>http://www.mobilemarketer.com/</t>
   </si>
   <si>
+    <t>What is Mobile Marketing? - Definition from Techopedia</t>
+  </si>
+  <si>
+    <t>https://www.techopedia.com/definition/14047/mobile-marketing</t>
+  </si>
+  <si>
+    <t>The Dominance of Mobile Marketing Is Complete - Entrepreneur</t>
+  </si>
+  <si>
+    <t>https://www.entrepreneur.com/article/290384</t>
+  </si>
+  <si>
     <t>Mobile Marketing News &amp; Trends | Marketing Land</t>
   </si>
   <si>
@@ -530,18 +566,6 @@
     <t>http://marketingland.com/library/mobile-marketing-news</t>
   </si>
   <si>
-    <t>What is Mobile Marketing? - Definition from Techopedia</t>
-  </si>
-  <si>
-    <t>https://www.techopedia.com/definition/14047/mobile-marketing</t>
-  </si>
-  <si>
-    <t>The Dominance of Mobile Marketing Is Complete - Entrepreneur</t>
-  </si>
-  <si>
-    <t>https://www.entrepreneur.com/article/290384</t>
-  </si>
-  <si>
     <t>Mobile Marketing | What is Mobile Marketing? - Marketing-Schools.org</t>
   </si>
   <si>
@@ -554,22 +578,52 @@
     <t>http://www.smartinsights.com/mobile-marketing/</t>
   </si>
   <si>
+    <t>MediaPost Publications - Mobile Marketing Daily</t>
+  </si>
+  <si>
+    <t>https://www.mediapost.com/publications/mobile-marketing-daily/</t>
+  </si>
+  <si>
+    <t>Vibes | Mobile Marketing Solutions</t>
+  </si>
+  <si>
+    <t>http://www.vibes.com/</t>
+  </si>
+  <si>
+    <t>- Mobile Marketing Engine</t>
+  </si>
+  <si>
+    <t>http://mobilemarketingengine.com/</t>
+  </si>
+  <si>
     <t>What is Mobile Marketing? (The Best Answer Ever!) - BuildFire</t>
   </si>
   <si>
     <t>https://buildfire.com/what-is-mobile-marketing/</t>
   </si>
   <si>
-    <t>News from the Mobile Payments, Marketing, and Technology Industries</t>
-  </si>
-  <si>
-    <t>http://mobilemarketingandtechnology.com/</t>
-  </si>
-  <si>
-    <t>MediaPost Publications - Mobile Marketing Daily</t>
-  </si>
-  <si>
-    <t>https://www.mediapost.com/publications/mobile-marketing-daily/</t>
+    <t>MobileMarketing.com - Mobile Text Marketing for Small Business</t>
+  </si>
+  <si>
+    <t>https://mobilemarketing.com/</t>
+  </si>
+  <si>
+    <t>8 Things to Know to Improve Your Mobile Marketing - R2i</t>
+  </si>
+  <si>
+    <t>http://www.r2integrated.com/r2insights/8-things-to-know-to-improve-your-mobile-marketing</t>
+  </si>
+  <si>
+    <t>Mobile Marketing Center - Ez Texting</t>
+  </si>
+  <si>
+    <t>https://www.eztexting.com/mobile-marketing-center</t>
+  </si>
+  <si>
+    <t>Mobile Marketing - Online Marketing Institute</t>
+  </si>
+  <si>
+    <t>https://www.onlinemarketinginstitute.org/classes/mobile-marketing/</t>
   </si>
   <si>
     <t>14 Mobile Marketing Tips That Drive Leads and Sales - Neil Patel</t>
@@ -578,28 +632,58 @@
     <t>http://neilpatel.com/blog/14-mobile-marketing-tips-to-drive-leads-and-sales/</t>
   </si>
   <si>
-    <t>MobileMarketing.com - Mobile Text Marketing for Small Business</t>
-  </si>
-  <si>
-    <t>https://mobilemarketing.com/</t>
-  </si>
-  <si>
-    <t>Mobile Marketing | LinkedIn</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/topic/mobile-marketing</t>
-  </si>
-  <si>
-    <t>Vibes | Mobile Marketing Solutions</t>
-  </si>
-  <si>
-    <t>http://www.vibes.com/</t>
-  </si>
-  <si>
-    <t>- Mobile Marketing Engine</t>
-  </si>
-  <si>
-    <t>http://mobilemarketingengine.com/</t>
+    <t>Mobile Marketing | Performics</t>
+  </si>
+  <si>
+    <t>http://www.performics.com/services/mobile-marketing/</t>
+  </si>
+  <si>
+    <t>8 Mobile Marketing Tips for Small Business - Business.com</t>
+  </si>
+  <si>
+    <t>https://www.business.com/articles/megan-totka-mobile-marketing/</t>
+  </si>
+  <si>
+    <t>Adobe Mobile Services</t>
+  </si>
+  <si>
+    <t>https://mobilemarketing.adobe.com/</t>
+  </si>
+  <si>
+    <t>Mobile Marketing | Digital Marketing Course - Digital Marketing Institute</t>
+  </si>
+  <si>
+    <t>https://digitalmarketinginstitute.com/students/courses/mobile-marketing</t>
+  </si>
+  <si>
+    <t>Mobile Marketing | Pilot Media Solutions</t>
+  </si>
+  <si>
+    <t>http://pilotmediasolutions.com/mobilemarketing</t>
+  </si>
+  <si>
+    <t>Mobile Marketing | Best Practices | Oracle Marketing Cloud</t>
+  </si>
+  <si>
+    <t>https://www.oracle.com/marketingcloud/resources/mobile-marketing.html</t>
+  </si>
+  <si>
+    <t>Mobile Marketing: Finding Your Customers No Matter Where They Are ...</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Mobile-Marketing-Finding-Customers-Matter/dp/0789739763</t>
+  </si>
+  <si>
+    <t>4 Mobile Marketing Strategies That Will Boost Engagement And Sales</t>
+  </si>
+  <si>
+    <t>http://www.forbes.com/sites/jaysondemers/2016/05/25/4-mobile-marketing-strategies-that-will-boost-engagement-and-sales/</t>
+  </si>
+  <si>
+    <t>Mobile Marketing Scorecard - FollowAnalytics</t>
+  </si>
+  <si>
+    <t>http://www.mobilemarketingscorecard.com/</t>
   </si>
   <si>
     <t>Mobile Marketing | Fishbowl - Data Analytics Solutions for the ...</t>
@@ -608,70 +692,10 @@
     <t>https://www.fishbowl.com/solutions/mobile/mobile-marketing/</t>
   </si>
   <si>
-    <t>Mobile Marketing Trends of 2017: The Sky's the Limit - Mapp</t>
-  </si>
-  <si>
-    <t>https://mapp.com/blog/mobile-marketing-trends-of-2017-skies-the-limit/</t>
-  </si>
-  <si>
-    <t>8 Things to Know to Improve Your Mobile Marketing - R2i</t>
-  </si>
-  <si>
-    <t>http://www.r2integrated.com/r2insights/8-things-to-know-to-improve-your-mobile-marketing</t>
-  </si>
-  <si>
-    <t>Mobile Marketing Center - Ez Texting</t>
-  </si>
-  <si>
-    <t>https://www.eztexting.com/mobile-marketing-center</t>
-  </si>
-  <si>
-    <t>Mobile Marketing - Online Marketing Institute</t>
-  </si>
-  <si>
-    <t>https://www.onlinemarketinginstitute.org/classes/mobile-marketing/</t>
-  </si>
-  <si>
-    <t>Travelport Digital Mobile Marketing | Travelport Digital</t>
-  </si>
-  <si>
-    <t>http://digital.travelport.com/solutions/travelport-digital-mobile-marketing</t>
-  </si>
-  <si>
-    <t>Mobile Marketing | Performics</t>
-  </si>
-  <si>
-    <t>http://www.performics.com/services/mobile-marketing/</t>
-  </si>
-  <si>
-    <t>Mobile Marketing | Best Practices | Oracle Marketing Cloud</t>
-  </si>
-  <si>
-    <t>https://www.oracle.com/marketingcloud/resources/mobile-marketing.html</t>
-  </si>
-  <si>
-    <t>4 Mobile Marketing Strategies That Will Boost Engagement And Sales</t>
-  </si>
-  <si>
-    <t>http://www.forbes.com/sites/jaysondemers/2016/05/25/4-mobile-marketing-strategies-that-will-boost-engagement-and-sales/</t>
-  </si>
-  <si>
-    <t>8 Mobile Marketing Tips for Small Business - Business.com</t>
-  </si>
-  <si>
-    <t>https://www.business.com/articles/megan-totka-mobile-marketing/</t>
-  </si>
-  <si>
-    <t>Adobe Mobile Services</t>
-  </si>
-  <si>
-    <t>https://mobilemarketing.adobe.com/</t>
-  </si>
-  <si>
-    <t>Amazon.com: Mobile Marketing (9780750667470): Alex Michael, Ben ...</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/Mobile-Marketing-Alex-Michael/dp/0750667478</t>
+    <t>Mobile Marketing Software Personalized Solutions - Salesforce.com</t>
+  </si>
+  <si>
+    <t>https://www.salesforce.com/products/marketing-cloud/channels/mobile-marketing-software/</t>
   </si>
   <si>
     <t>Google search results for: Mobile internet</t>
@@ -680,7 +704,7 @@
     <t>Shop for Mobile internet on Google</t>
   </si>
   <si>
-    <t>https://www.google.com/search?q=Mobile+internet&amp;biw=1050&amp;bih=549&amp;source=univ&amp;tbm=shop&amp;tbo=u&amp;sa=X&amp;ved=0ahUKEwjc86iw0bvTAhXD5SYKHUkEDfcQsxgIIw</t>
+    <t>https://www.google.com/search?q=Mobile+internet&amp;biw=1050&amp;bih=548&amp;source=univ&amp;tbm=shop&amp;tbo=u&amp;sa=X&amp;ved=0ahUKEwi5y7H6o7zTAhWKdSYKHXJCC1gQsxgIIg</t>
   </si>
   <si>
     <t>Mobile Hotspots, Mobile Internet, MiFi Jetpacks | Verizon Wireless</t>
@@ -719,18 +743,18 @@
     <t>https://support.t-mobile.com/community/phones-tablets-devices/mobile-internet</t>
   </si>
   <si>
+    <t>Mobile Internet Hotspots &amp; Smartphone Wifi Internet Access | T-Mobile</t>
+  </si>
+  <si>
+    <t>https://www.t-mobile.com/shop/addons/Services/information.aspx?PAsset=InternetEmail&amp;tp=Svc_Tab_HotSpot&amp;tsp</t>
+  </si>
+  <si>
     <t>Company Information | T-Mobile's Broadband Internet Access Services</t>
   </si>
   <si>
     <t>http://www.t-mobile.com/company/company-info/consumer/internet-services.html</t>
   </si>
   <si>
-    <t>Mobile Internet Hotspots &amp; Smartphone Wifi Internet Access | T-Mobile</t>
-  </si>
-  <si>
-    <t>https://www.t-mobile.com/shop/addons/Services/information.aspx?PAsset=InternetEmail&amp;tp=Svc_Tab_HotSpot&amp;tsp</t>
-  </si>
-  <si>
     <t>RV Mobile Internet Resource Center</t>
   </si>
   <si>
@@ -743,7 +767,7 @@
     <t>http://www.netzero.net/start/showAllDevices.do?wls_rsf=1</t>
   </si>
   <si>
-    <t>https://www.google.com/search?q=Mobile+internet&amp;biw=1050&amp;bih=549&amp;source=univ&amp;tbm=shop&amp;tbo=u&amp;sa=X&amp;ved=0ahUKEwix4Kyy0bvTAhWGSiYKHTNsDKM4ChCzGAgj</t>
+    <t>https://www.google.com/search?q=Mobile+internet&amp;biw=1050&amp;bih=548&amp;source=univ&amp;tbm=shop&amp;tbo=u&amp;sa=X&amp;ved=0ahUKEwie5PX7o7zTAhUFMSYKHWblBoQ4ChCzGAgi</t>
   </si>
   <si>
     <t>Mobile Web - Wikipedia</t>
@@ -764,30 +788,30 @@
     <t>https://www.lifewire.com/mobile-internet-access-comparison-2378207</t>
   </si>
   <si>
+    <t>Mobile Internet - Cisco</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/c/en/us/solutions/service-provider/mobile-internet/index.html</t>
+  </si>
+  <si>
+    <t>T-Mobile $30 Prepaid Mobile Internet On-Demand Pass (Email ...</t>
+  </si>
+  <si>
+    <t>https://www.walmart.com/ip/T-Mobile-30-Prepaid-Mobile-Internet-On-Demand-Pass-Email-Delivery/33871029</t>
+  </si>
+  <si>
+    <t>The countries with the world's fastest mobile internet - Quartz</t>
+  </si>
+  <si>
+    <t>https://qz.com/915726/the-countries-with-the-worlds-fastest-mobile-internet/</t>
+  </si>
+  <si>
     <t>NetZero: Broadband Internet | Mobile Broadband | DSL | Dial-Up</t>
   </si>
   <si>
     <t>http://www.netzero.net/</t>
   </si>
   <si>
-    <t>T-Mobile $30 Prepaid Mobile Internet On-Demand Pass (Email ...</t>
-  </si>
-  <si>
-    <t>https://www.walmart.com/ip/T-Mobile-30-Prepaid-Mobile-Internet-On-Demand-Pass-Email-Delivery/33871029</t>
-  </si>
-  <si>
-    <t>Mobile Internet - Cisco</t>
-  </si>
-  <si>
-    <t>http://www.cisco.com/c/en/us/solutions/service-provider/mobile-internet/index.html</t>
-  </si>
-  <si>
-    <t>The countries with the world's fastest mobile internet - Quartz</t>
-  </si>
-  <si>
-    <t>https://qz.com/915726/the-countries-with-the-worlds-fastest-mobile-internet/</t>
-  </si>
-  <si>
     <t>Mobile Hot Spot &amp; Internet | Cellular PlusThe Right Device at Verizon ...</t>
   </si>
   <si>
@@ -806,9 +830,6 @@
     <t>http://money.cnn.com/2016/12/14/technology/internet-availability-speed-comparison/</t>
   </si>
   <si>
-    <t>https://www.google.com/search?q=Mobile+internet&amp;biw=1050&amp;bih=549&amp;source=univ&amp;tbm=shop&amp;tbo=u&amp;sa=X&amp;ved=0ahUKEwjEvMCz0bvTAhVBPCYKHQwJBvY4FBCzGAgj</t>
-  </si>
-  <si>
     <t>Ethiopia partially restores mobile internet after 2 month shutdown ...</t>
   </si>
   <si>
@@ -869,7 +890,7 @@
     <t>https://www.bell.ca/Mobility/Mobile-Internet-Devices-listing</t>
   </si>
   <si>
-    <t>https://www.google.com/search?q=Mobile+internet&amp;biw=1050&amp;bih=549&amp;source=univ&amp;tbm=shop&amp;tbo=u&amp;sa=X&amp;ved=0ahUKEwiHxtO00bvTAhXE6SYKHfB9CkY4HhCzGAgj</t>
+    <t>https://www.google.com/search?q=Mobile+internet&amp;biw=1050&amp;bih=548&amp;source=univ&amp;tbm=shop&amp;tbo=u&amp;sa=X&amp;ved=0ahUKEwjv-ZX-o7zTAhVGKCYKHQyiCoE4HhCzGAgi</t>
   </si>
   <si>
     <t>Mobile Internet ETF Alternative | Mobile Internet Stocks - Motif</t>
@@ -1075,322 +1096,322 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="B43" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>53</v>
+        <v>85</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B47" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>65</v>
+        <v>89</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>94</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="B53" t="s">
-        <v>76</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1408,7 +1429,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3">
@@ -1437,10 +1458,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8">
@@ -1453,66 +1474,66 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17">
@@ -1533,10 +1554,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20">
@@ -1549,306 +1570,306 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>102</v>
+        <v>126</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="B37" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>109</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="B41" t="s">
-        <v>111</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B44" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>124</v>
       </c>
       <c r="B45" t="s">
-        <v>72</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="B46" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="B47" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="B48" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="B50" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="B51" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>128</v>
+        <v>63</v>
       </c>
       <c r="B52" t="s">
-        <v>129</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="B54" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="B56" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>138</v>
+        <v>75</v>
       </c>
       <c r="B58" t="s">
-        <v>139</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1866,7 +1887,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3">
@@ -1879,394 +1900,394 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="B17" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B20" t="s">
-        <v>152</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="B21" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="B22" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="B23" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="B24" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="B25" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B27" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
       <c r="B28" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="B29" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="B30" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="B31" t="s">
-        <v>174</v>
+        <v>182</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="B32" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B33" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
       <c r="B34" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="B35" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>183</v>
+        <v>191</v>
       </c>
       <c r="B36" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="B37" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="B38" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B39" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="B40" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="B41" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="B42" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B43" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="B44" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="B45" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="B46" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="B47" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="B48" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="B49" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="B50" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="B51" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="B52" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="B53" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2276,7 +2297,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2284,7 +2305,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3">
@@ -2297,458 +2318,450 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B5" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B6" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B7" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="B9" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B10" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B11" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B12" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B13" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="B14" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B15" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="B16" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B17" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B18" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="B19" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B20" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="B21" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="B22" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="B23" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="B24" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="B25" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="B26" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="B27" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="B28" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="B29" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>243</v>
+        <v>251</v>
       </c>
       <c r="B30" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="B31" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>247</v>
+        <v>255</v>
       </c>
       <c r="B32" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="B33" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="B34" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="B35" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="B36" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>257</v>
+        <v>265</v>
       </c>
       <c r="B37" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="B38" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="B39" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>220</v>
+        <v>271</v>
       </c>
       <c r="B40" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="B41" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="B42" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="B43" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="B44" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="B45" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="B46" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="B47" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="B48" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="B49" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>282</v>
+        <v>228</v>
       </c>
       <c r="B50" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>220</v>
+        <v>292</v>
       </c>
       <c r="B51" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="B52" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="B53" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="B54" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="B55" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="B56" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="B57" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="B58" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="B59" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="B60" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
-        <v>303</v>
-      </c>
-      <c r="B61" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>